<commit_message>
Changed table item names
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Source_Code/proman-project/proman-batch/src/test/java/com/nablarch/example/proman/batch/project/ExportProjectsInPeriodActionRequestTest.xlsx
+++ b/en/Sample_Project/Source_Code/proman-project/proman-batch/src/test/java/com/nablarch/example/proman/batch/project/ExportProjectsInPeriodActionRequestTest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BE7113-A935-4BDF-ACAC-20A1003D21BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE4534-CADB-4391-8716-A14B5513ECDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="489" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="489" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setUpDb" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,15 @@
     <definedName name="Excel_BuiltIn_Sheet_Title_2">"testSelectUserGroups"</definedName>
     <definedName name="データ型">[1]データ!$A$2:$A$22</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,16 +133,7 @@
     <t>client_id</t>
   </si>
   <si>
-    <t>project_manager</t>
-  </si>
-  <si>
-    <t>project_leader</t>
-  </si>
-  <si>
     <t>note</t>
-  </si>
-  <si>
-    <t>sales</t>
   </si>
   <si>
     <t>version_no</t>
@@ -1476,6 +1475,15 @@
       </rPr>
       <t>Project name 2</t>
     </r>
+  </si>
+  <si>
+    <t>pm_kanji_name</t>
+  </si>
+  <si>
+    <t>pl_kanji_name</t>
+  </si>
+  <si>
+    <t>sales_amount</t>
   </si>
 </sst>
 </file>
@@ -2427,7 +2435,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="29.25">
       <c r="A1" s="37" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2444,7 +2452,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2460,7 +2468,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
@@ -2482,7 +2490,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="29.25">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2549,89 +2557,89 @@
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1" ht="21">
       <c r="A4" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="J4" s="39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="17" customFormat="1" ht="12.75">
@@ -2674,7 +2682,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -2683,7 +2691,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -2716,112 +2724,112 @@
         <v>26</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="L11" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="14.25">
       <c r="A12" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="E12" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="F12" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="G12" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="H12" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="J12" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="K12" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="L12" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="M12" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="N12" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25">
       <c r="A13" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="F13" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="25" t="s">
+      <c r="H13" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="J13" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="K13" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="24" t="s">
+      <c r="L13" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="M13" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="N13" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="41" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -2855,101 +2863,101 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="F21" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="G21" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="H21" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="I21" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="J21" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="42" t="s">
+      <c r="K21" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="L21" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="M21" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="K21" s="42" t="s">
+      <c r="N21" s="42" t="s">
         <v>123</v>
-      </c>
-      <c r="L21" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M21" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="N21" s="42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="28"/>
       <c r="B22" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N22" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="29.25">
       <c r="A24" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -2969,7 +2977,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -2978,7 +2986,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -3011,156 +3019,156 @@
         <v>26</v>
       </c>
       <c r="I27" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="L27" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.25">
       <c r="A28" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="F28" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="J28" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="K28" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I28" s="24" t="s">
+      <c r="L28" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="J28" s="24" t="s">
+      <c r="M28" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="N28" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="L28" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="14.25">
       <c r="A29" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="E29" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="F29" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="H29" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="25" t="s">
+      <c r="J29" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K29" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H29" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="24" t="s">
+      <c r="L29" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="M29" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="K29" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="L29" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="M29" s="25" t="s">
-        <v>99</v>
-      </c>
       <c r="N29" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.25">
       <c r="A30" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B30" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="G30" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="25" t="s">
+      <c r="H30" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="K30" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="H30" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I30" s="24" t="s">
+      <c r="L30" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="M30" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K30" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L30" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="M30" s="25" t="s">
-        <v>111</v>
-      </c>
       <c r="N30" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3169,7 +3177,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3194,143 +3202,143 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B38" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="F38" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="G38" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="H38" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="I38" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="42" t="s">
+      <c r="J38" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H38" s="42" t="s">
+      <c r="K38" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="I38" s="42" t="s">
+      <c r="L38" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="J38" s="42" t="s">
+      <c r="M38" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="K38" s="42" t="s">
+      <c r="N38" s="42" t="s">
         <v>123</v>
-      </c>
-      <c r="L38" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M38" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="N38" s="42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="27"/>
       <c r="B39" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I39" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M39" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N39" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="14.25">
       <c r="A40" s="28"/>
       <c r="B40" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J40" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N40" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="29.25">
       <c r="A42" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -3350,7 +3358,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3359,7 +3367,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3392,283 +3400,283 @@
         <v>26</v>
       </c>
       <c r="I45" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K45" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J45" s="11" t="s">
+      <c r="L45" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="M45" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="K45" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M45" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="14.25">
       <c r="A46" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I46" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="J46" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K46" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L46" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="24" t="s">
+      <c r="M46" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="K46" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="L46" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="M46" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="N46" s="9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="14.25">
       <c r="A47" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C47" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H47" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="H47" s="25" t="s">
-        <v>37</v>
-      </c>
       <c r="I47" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="J47" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K47" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="L47" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="J47" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="K47" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="L47" s="25" t="s">
-        <v>98</v>
-      </c>
       <c r="M47" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="14.25">
       <c r="A48" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" s="25" t="s">
-        <v>43</v>
-      </c>
       <c r="H48" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I48" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J48" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K48" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L48" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="J48" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="K48" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L48" s="25" t="s">
-        <v>110</v>
-      </c>
       <c r="M48" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="14.25">
       <c r="A49" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B49" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="G49" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H49" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>150</v>
-      </c>
       <c r="J49" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K49" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L49" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M49" s="25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="14.25">
       <c r="A50" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F50" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G50" s="36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J50" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K50" s="24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L50" s="32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M50" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N50" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="14.25">
       <c r="A51" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G51" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H51" s="25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I51" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="J51" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="K51" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="L51" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="J51" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="K51" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="L51" s="25" t="s">
+      <c r="M51" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N51" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="M51" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="N51" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3676,7 +3684,7 @@
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -3686,7 +3694,7 @@
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3711,267 +3719,267 @@
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B58" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="42" t="s">
+      <c r="F58" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="42" t="s">
+      <c r="G58" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="H58" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F58" s="42" t="s">
+      <c r="I58" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="G58" s="42" t="s">
+      <c r="J58" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H58" s="42" t="s">
+      <c r="K58" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="I58" s="42" t="s">
+      <c r="L58" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="J58" s="42" t="s">
+      <c r="M58" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="K58" s="42" t="s">
+      <c r="N58" s="42" t="s">
         <v>123</v>
-      </c>
-      <c r="L58" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="M58" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="N58" s="42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="27"/>
       <c r="B59" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H59" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I59" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J59" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L59" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M59" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N59" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="14.25">
       <c r="A60" s="27"/>
       <c r="B60" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E60" s="24" t="s">
         <v>11</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J60" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K60" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L60" s="24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M60" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N60" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O60" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="27"/>
       <c r="B61" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I61" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J61" s="30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K61" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L61" s="30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N61" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="27"/>
       <c r="B62" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D62" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J62" s="30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K62" s="30" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N62" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="28"/>
       <c r="B63" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J63" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K63" s="30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L63" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M63" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N63" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>